<commit_message>
multithreading for pedestals, compresed options added
</commit_message>
<xml_diff>
--- a/new_macros/Runs_list.xlsx
+++ b/new_macros/Runs_list.xlsx
@@ -149,17 +149,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>